<commit_message>
fix message in admin main page , add button in show_student_info in admin_bot, delete one message in show_teachers in user_bot
</commit_message>
<xml_diff>
--- a/data/lastVersion_student.xlsx
+++ b/data/lastVersion_student.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>شماره ردیف</t>
   </si>
@@ -64,7 +64,7 @@
     <t>زمان انتخاب شده چهارم</t>
   </si>
   <si>
-    <t>سید علی</t>
+    <t>سد علی</t>
   </si>
   <si>
     <t>کارشناسی</t>
@@ -79,13 +79,13 @@
     <t>تهران</t>
   </si>
   <si>
-    <t>شسیبشسبمکنتبثس</t>
+    <t>من استاد راهنما ام خیلی خوبه</t>
   </si>
   <si>
     <t>۰۹۱۹</t>
   </si>
   <si>
-    <t>اکبر یوسفی</t>
+    <t>علیرضا باقری</t>
   </si>
   <si>
     <t>شنبه ها بعد از ظهر</t>
@@ -97,10 +97,19 @@
     <t>9000</t>
   </si>
   <si>
-    <t>حسن حسنی</t>
+    <t>ایوب حسنی</t>
   </si>
   <si>
     <t>یکشنبه</t>
+  </si>
+  <si>
+    <t>محمد</t>
+  </si>
+  <si>
+    <t>مهندسی عمران</t>
+  </si>
+  <si>
+    <t>س</t>
   </si>
 </sst>
 </file>
@@ -668,13 +677,19 @@
       <c r="A7" s="8">
         <v>3</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="E7" s="10"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="H7" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>

</xml_diff>